<commit_message>
Correlation Anaylsis with moving window
</commit_message>
<xml_diff>
--- a/results/persons_correlation.xlsx
+++ b/results/persons_correlation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>PAR</t>
   </si>
@@ -44,12 +44,6 @@
   </si>
   <si>
     <t>preds_preles</t>
-  </si>
-  <si>
-    <t>preds_nn_obs</t>
-  </si>
-  <si>
-    <t>preds_nn_preles</t>
   </si>
 </sst>
 </file>
@@ -407,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -444,10 +438,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.8245308223245011</v>
+        <v>0.8245308223245013</v>
       </c>
       <c r="C2">
-        <v>0.7789893595035465</v>
+        <v>0.7789893595035462</v>
       </c>
       <c r="D2">
         <v>0.6737040251204729</v>
@@ -459,7 +453,7 @@
         <v>0.6546117580525407</v>
       </c>
       <c r="G2">
-        <v>-0.06296415060617208</v>
+        <v>-0.0629641506061721</v>
       </c>
       <c r="H2">
         <v>-0.8871399039473178</v>
@@ -479,13 +473,13 @@
         <v>0.8118842377318201</v>
       </c>
       <c r="D3">
-        <v>0.7530053152991975</v>
+        <v>0.7530053152991972</v>
       </c>
       <c r="E3">
         <v>-0.1080954291659264</v>
       </c>
       <c r="F3">
-        <v>0.8098869303437772</v>
+        <v>0.8098869303437776</v>
       </c>
       <c r="G3">
         <v>-0.2188794593540277</v>
@@ -495,64 +489,6 @@
       </c>
       <c r="I3" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>0.8397204248574501</v>
-      </c>
-      <c r="C4">
-        <v>0.7957422581097578</v>
-      </c>
-      <c r="D4">
-        <v>0.6931961562047989</v>
-      </c>
-      <c r="E4">
-        <v>-0.0762051016595818</v>
-      </c>
-      <c r="F4">
-        <v>0.6647966284064346</v>
-      </c>
-      <c r="G4">
-        <v>-0.06678784117159534</v>
-      </c>
-      <c r="H4">
-        <v>-0.9036173873340005</v>
-      </c>
-      <c r="I4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>0.8066961343706949</v>
-      </c>
-      <c r="C5">
-        <v>0.812734110817229</v>
-      </c>
-      <c r="D5">
-        <v>0.7532667922325567</v>
-      </c>
-      <c r="E5">
-        <v>-0.1083867442033462</v>
-      </c>
-      <c r="F5">
-        <v>0.8117781811258309</v>
-      </c>
-      <c r="G5">
-        <v>-0.2193992687211848</v>
-      </c>
-      <c r="H5">
-        <v>-0.8224663155948282</v>
-      </c>
-      <c r="I5" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>